<commit_message>
Spring Hibernate Integration in backend project
</commit_message>
<xml_diff>
--- a/ErrorPage and solutions.xlsx
+++ b/ErrorPage and solutions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>S.No</t>
   </si>
@@ -129,6 +129,16 @@
   </si>
   <si>
     <t xml:space="preserve">value couldn't return from backend </t>
+  </si>
+  <si>
+    <t>17/102016</t>
+  </si>
+  <si>
+    <t>Spring Hibernate configuration</t>
+  </si>
+  <si>
+    <t>INFO: Using DataSource [org.springframework.jdbc.datasource.DriverManagerDataSource@31d7b7bf] of Hibernate SessionFactory for HibernateTransactionManager
+Exception in thread "main" javax.persistence.PersistenceException: org.hibernate.PersistentObjectException: detached entity passed to persist: com.niit.Backend.Model.ProductBean</t>
   </si>
 </sst>
 </file>
@@ -554,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +588,7 @@
     <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -706,13 +717,25 @@
       <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="E6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>

</xml_diff>